<commit_message>
Cleaned code, added df cleaning functions, and modeling
</commit_message>
<xml_diff>
--- a/ConnorHaas/Variable Analysis.xlsx
+++ b/ConnorHaas/Variable Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conma\Desktop\NYCDSA\Machine Learning\Machine_Learning_Project\ConnorHaas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706BC759-9FCD-49A7-AB78-D90882E4A768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37299AC6-3ED2-4B1C-97D0-58C9EC7BF6B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88992439-1954-4851-A431-0E6797FC405A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="125">
   <si>
     <t>Id</t>
   </si>
@@ -394,13 +394,25 @@
   </si>
   <si>
     <t>does it matter? Mar-Aug higher dist, maybe base on season?</t>
+  </si>
+  <si>
+    <t>Log, boxcox, kfolds? - heavily weighted</t>
+  </si>
+  <si>
+    <t>Lotfrontage</t>
+  </si>
+  <si>
+    <t>lotarea</t>
+  </si>
+  <si>
+    <t>lotshape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,12 +430,6 @@
     <font>
       <sz val="8"/>
       <color rgb="FFD84315"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -481,19 +487,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,526 +811,951 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971854EF-8730-4BAF-BEF9-3BD8011E105A}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="57.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B4" s="4">
+        <v>82.26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B5" s="4">
+        <v>100</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B6" s="2">
+        <v>100</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B7" s="2">
+        <v>6.23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B8" s="4">
+        <v>100</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B9" s="2">
+        <v>100</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B10" s="2">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B11" s="2">
+        <v>100</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B12" s="2">
+        <v>100</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B13" s="3">
+        <v>100</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B14" s="2">
+        <v>100</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B15" s="2">
+        <v>100</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B16" s="2">
+        <v>100</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B17" s="4">
+        <v>100</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B18" s="4">
+        <v>100</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B19" s="4">
+        <v>100</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B21" s="3">
+        <v>100</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B22" s="2">
+        <v>100</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B23" s="2">
+        <v>100</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B24" s="2">
+        <v>100</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B25" s="2">
+        <v>100</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B26" s="2">
+        <v>99.45</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B27" s="4">
+        <v>99.45</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B28" s="2">
+        <v>100</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B29" s="2">
+        <v>100</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B30" s="2">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="B31" s="2">
+        <v>97.46</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="B32" s="2">
+        <v>97.46</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B33" s="2">
+        <v>97.39</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B34" s="2">
+        <v>97.46</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B35" s="2">
+        <v>100</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B36" s="2">
+        <v>97.39</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B37" s="2">
+        <v>100</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B38" s="2">
+        <v>100</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="B39" s="4">
+        <v>100</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="B40" s="4">
+        <v>100</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B41" s="2">
+        <v>100</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="6">
-        <v>100</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="6" t="s">
+      <c r="B42" s="4">
+        <v>100</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="2">
         <v>99.93</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="C43" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="5">
-        <v>100</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B44" s="4">
+        <v>100</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D44" t="s">
         <v>99</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="5">
-        <v>100</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B45" s="4">
+        <v>100</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D45" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="6">
-        <v>100</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="B46" s="2">
+        <v>100</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="5">
-        <v>100</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="7" t="s">
+      <c r="B47" s="4">
+        <v>100</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="5">
-        <v>100</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="B48" s="4">
+        <v>100</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D48" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
+      <c r="E48" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="6">
-        <v>100</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" s="6" t="s">
+      <c r="B49" s="2">
+        <v>100</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+      <c r="E49" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="5">
-        <v>100</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="B50" s="4">
+        <v>100</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D50" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="E50" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="5">
-        <v>100</v>
-      </c>
-      <c r="C51" s="5" t="s">
+      <c r="B51" s="4">
+        <v>100</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D51" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="5">
-        <v>100</v>
-      </c>
-      <c r="C52" s="5" t="s">
+      <c r="B52" s="4">
+        <v>100</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D52" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="6">
-        <v>100</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="6" t="s">
+      <c r="B53" s="5">
+        <v>100</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="6">
-        <v>100</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" s="6" t="s">
+      <c r="B54" s="4">
+        <v>100</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="4">
-        <v>100</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D55" s="3" t="s">
+      <c r="B55" s="2">
+        <v>100</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="6">
-        <v>100</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" s="6" t="s">
+      <c r="B56" s="5">
+        <v>100</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="5">
-        <v>100</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="B57" s="4">
+        <v>100</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>52.73</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
+      <c r="C58" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="5">
         <v>94.45</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D59" s="6" t="s">
+      <c r="C59" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>94.45</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61" s="2">
         <v>94.45</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="3" t="s">
+      <c r="C61" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>61</v>
       </c>
@@ -1337,25 +1765,25 @@
       <c r="C62" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="4">
-        <v>100</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B63" s="2">
+        <v>100</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -1365,46 +1793,46 @@
       <c r="C64" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="2">
         <v>94.45</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D65" s="3" t="s">
+      <c r="C65" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="6">
-        <v>100</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="6" t="s">
+      <c r="B66" s="2">
+        <v>100</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="5">
-        <v>100</v>
-      </c>
-      <c r="C67" s="5" t="s">
+      <c r="B67" s="4">
+        <v>100</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D67" t="s">
@@ -1412,13 +1840,13 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="5">
-        <v>100</v>
-      </c>
-      <c r="C68" s="5" t="s">
+      <c r="B68" s="4">
+        <v>100</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D68" t="s">
@@ -1426,94 +1854,94 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="6">
-        <v>100</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D69" s="6" t="s">
+      <c r="B69" s="2">
+        <v>100</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="6">
-        <v>100</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D70" s="6" t="s">
+      <c r="B70" s="2">
+        <v>100</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="6">
-        <v>100</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D71" s="6" t="s">
+      <c r="B71" s="2">
+        <v>100</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="6">
-        <v>100</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D72" s="6" t="s">
+      <c r="B72" s="5">
+        <v>100</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <v>0.47</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="5">
         <v>19.239999999999998</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D74" s="6" t="s">
+      <c r="C74" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>3.69</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D75" t="s">
@@ -1521,13 +1949,13 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="3">
-        <v>100</v>
-      </c>
-      <c r="C76" s="3" t="s">
+      <c r="B76" s="2">
+        <v>100</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D76" t="s">
@@ -1535,13 +1963,13 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B77">
-        <v>100</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="B77" s="2">
+        <v>100</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D77" t="s">
@@ -1549,13 +1977,13 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B78">
-        <v>100</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B78" s="2">
+        <v>100</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D78" t="s">
@@ -1563,30 +1991,30 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="6">
-        <v>100</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D79" s="6" t="s">
+      <c r="B79" s="5">
+        <v>100</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="6">
-        <v>100</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D80" s="6" t="s">
+      <c r="B80" s="5">
+        <v>100</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1602,7 +2030,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>